<commit_message>
Update detail absensi polda
</commit_message>
<xml_diff>
--- a/public/template/excel/absensi.xlsx
+++ b/public/template/excel/absensi.xlsx
@@ -30,10 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
-  <si>
-    <t>HARI/TGL :</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>POLDA ACEH</t>
   </si>
@@ -135,13 +132,25 @@
   </si>
   <si>
     <t>POLDA KALTARA</t>
+  </si>
+  <si>
+    <t>Senin, 18 Oktober 2021</t>
+  </si>
+  <si>
+    <t>NOMOR</t>
+  </si>
+  <si>
+    <t>POLDA</t>
+  </si>
+  <si>
+    <t>STATUS PENGIRIMAN LAPORAN HARIAN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,11 +185,6 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -196,27 +200,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -233,23 +222,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -258,27 +252,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="1"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -609,255 +583,356 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="178" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="90.109375" style="6" customWidth="1"/>
-    <col min="3" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="9.6640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="36.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="61.77734375" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="C3" s="10"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="C6" s="10"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="C7" s="10"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="C8" s="10"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="10"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="10"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="5"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="C11" s="10"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="5"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="5"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="C12" s="10"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>11</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="10"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="C14" s="10"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>13</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="5"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="5"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="C15" s="10"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>14</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="5"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="C16" s="10"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>15</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="5"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="C17" s="10"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>16</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="5"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="C18" s="10"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>17</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="10"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>18</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="10"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>19</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="10"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>20</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="10"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>21</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="10"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>22</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="10"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>23</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="10"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>24</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="10"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>25</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="10"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
+        <v>26</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="10"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>27</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="10"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
+        <v>28</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="5"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="C30" s="10"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <v>29</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="5"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="5"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="5"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="5"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="C31" s="10"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
+        <v>30</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="10"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <v>31</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="10"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
+        <v>32</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="10"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <v>33</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="10"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
         <v>34</v>
       </c>
-      <c r="B23" s="5"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="5"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="5"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="5"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="5"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="5"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="5"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" s="5"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" s="5"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" s="5"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="B36" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="5"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B34" s="5"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" s="5"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" s="5"/>
+      <c r="C36" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:B1048576">
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="BELUM MENGIRIMKAN DATA">
-      <formula>NOT(ISERROR(SEARCH("BELUM MENGIRIMKAN DATA",B3)))</formula>
+  <conditionalFormatting sqref="B37:B1048576">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="BELUM MENGIRIMKAN DATA">
+      <formula>NOT(ISERROR(SEARCH("BELUM MENGIRIMKAN DATA",B37)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"SUDAH MENGIRIMKAN DATA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
-      <formula>"BELUM MENGIRIMKAN DATA"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4">
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="BELUM MENGIRIMKAN DATA">
-      <formula>NOT(ISERROR(SEARCH("BELUM MENGIRIMKAN DATA",B4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B36">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
       <formula>"BELUM MENGIRIMKAN DATA"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>